<commit_message>
gui copied from nsternie/live_telemetry
Copied over some of my previous work from the live telem project as a framework for this gui
</commit_message>
<xml_diff>
--- a/board_design/Prop Support Board REV A Mastersheet.xlsx
+++ b/board_design/Prop Support Board REV A Mastersheet.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexh\OneDrive\Desktop\masa\prop_support_board\board_design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61e783b3884bd71f/Desktop/masa/prop_support_board/board_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="6_{42469BF5-BBA4-42B4-BC35-A4CF2E66CA7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{65C61123-ECA5-433B-AD4A-F1970DA66017}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="6_{8AA88C21-F14F-4B80-883F-7B5DEDC5B43F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{7AB7F95E-2497-45C1-BFFD-6FA2681D3416}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2B8E7E47-A030-46FA-978B-DCE8E3A55E06}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{2B8E7E47-A030-46FA-978B-DCE8E3A55E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Budget" sheetId="1" r:id="rId1"/>
     <sheet name="Bill of Materials" sheetId="3" r:id="rId2"/>
-    <sheet name="To Do" sheetId="2" r:id="rId3"/>
+    <sheet name="Calculations" sheetId="4" r:id="rId3"/>
+    <sheet name="To Do" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="427">
   <si>
     <t>ADC</t>
   </si>
@@ -1215,6 +1216,99 @@
   </si>
   <si>
     <t>S1, S2, S3, S4, S5, S6, S7, S8</t>
+  </si>
+  <si>
+    <t>Voltage Divider</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>Trace Calculator</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Ambient Temperature</t>
+  </si>
+  <si>
+    <t>Temperature Rise</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>Voltage Drop</t>
+  </si>
+  <si>
+    <t>Power Loss</t>
+  </si>
+  <si>
+    <t>Trace Calc constants</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>oz</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>mils</t>
+  </si>
+  <si>
+    <t>ohm</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>mil</t>
+  </si>
+  <si>
+    <t>mil^2</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>fix trace calc</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1251,8 +1345,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1340,24 +1446,255 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1366,31 +1703,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1482,8 +1842,8 @@
     <tableColumn id="1" xr3:uid="{F721E539-36B1-4AFD-8013-C15CAE125017}" name="Item"/>
     <tableColumn id="2" xr3:uid="{6FFD5F0E-8357-4490-9209-8CECC2BB6BB4}" name="Qty"/>
     <tableColumn id="3" xr3:uid="{C8079886-0D4D-4220-BE0B-BB97FEE70D2F}" name="Reference(s)" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{FD875F74-2C17-45BF-AD0A-5DFD3C9C56B5}" name="Value" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{D4638B41-5897-415B-A9E3-9573EA37E92B}" name="LibPart" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{FD875F74-2C17-45BF-AD0A-5DFD3C9C56B5}" name="Value" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D4638B41-5897-415B-A9E3-9573EA37E92B}" name="LibPart" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{7503C650-F12D-489D-8391-61865B357F48}" name="Footprint"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1789,8 +2149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CEAB82-77BA-4993-A757-2BBA210F51AE}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1801,15 +2161,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
@@ -2061,74 +2421,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37099C8B-24F3-4159-BF12-17F86D08A509}">
   <dimension ref="A1:N235"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D205" sqref="D205"/>
+    <sheetView topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="B236" sqref="B236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="15.5234375" customWidth="1"/>
-    <col min="3" max="3" width="43.26171875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18" style="4" customWidth="1"/>
-    <col min="5" max="5" width="34.68359375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.26171875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.68359375" style="2" customWidth="1"/>
     <col min="6" max="6" width="78.26171875" customWidth="1"/>
     <col min="7" max="14" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="20">
         <v>43554.648553240739</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="24">
         <v>183</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -2143,13 +2503,13 @@
       <c r="B9" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F9" t="s">
@@ -2181,13 +2541,13 @@
       </c>
     </row>
     <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F10" t="s">
@@ -2198,13 +2558,13 @@
       </c>
     </row>
     <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F11" t="s">
@@ -2212,13 +2572,13 @@
       </c>
     </row>
     <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F12" t="s">
@@ -2226,13 +2586,13 @@
       </c>
     </row>
     <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F13" t="s">
@@ -2240,13 +2600,13 @@
       </c>
     </row>
     <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F14" t="s">
@@ -2254,13 +2614,13 @@
       </c>
     </row>
     <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F15" t="s">
@@ -2268,13 +2628,13 @@
       </c>
     </row>
     <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F16" t="s">
@@ -2282,13 +2642,13 @@
       </c>
     </row>
     <row r="17" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F17" t="s">
@@ -2296,13 +2656,13 @@
       </c>
     </row>
     <row r="18" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F18" t="s">
@@ -2310,13 +2670,13 @@
       </c>
     </row>
     <row r="19" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F19" t="s">
@@ -2324,13 +2684,13 @@
       </c>
     </row>
     <row r="20" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F20" t="s">
@@ -2338,13 +2698,13 @@
       </c>
     </row>
     <row r="21" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F21" t="s">
@@ -2352,13 +2712,13 @@
       </c>
     </row>
     <row r="22" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F22" t="s">
@@ -2366,13 +2726,13 @@
       </c>
     </row>
     <row r="23" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F23" t="s">
@@ -2380,13 +2740,13 @@
       </c>
     </row>
     <row r="24" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F24" t="s">
@@ -2394,13 +2754,13 @@
       </c>
     </row>
     <row r="25" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F25" t="s">
@@ -2408,13 +2768,13 @@
       </c>
     </row>
     <row r="26" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F26" t="s">
@@ -2422,13 +2782,13 @@
       </c>
     </row>
     <row r="27" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F27" t="s">
@@ -2439,13 +2799,13 @@
       </c>
     </row>
     <row r="28" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F28" t="s">
@@ -2453,13 +2813,13 @@
       </c>
     </row>
     <row r="29" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F29" t="s">
@@ -2467,13 +2827,13 @@
       </c>
     </row>
     <row r="30" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F30" t="s">
@@ -2484,13 +2844,13 @@
       </c>
     </row>
     <row r="31" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F31" t="s">
@@ -2501,13 +2861,13 @@
       </c>
     </row>
     <row r="32" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F32" t="s">
@@ -2518,13 +2878,13 @@
       </c>
     </row>
     <row r="33" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F33" t="s">
@@ -2535,13 +2895,13 @@
       </c>
     </row>
     <row r="34" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F34" t="s">
@@ -2552,13 +2912,13 @@
       </c>
     </row>
     <row r="35" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F35" t="s">
@@ -2569,13 +2929,13 @@
       </c>
     </row>
     <row r="36" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F36" t="s">
@@ -2586,13 +2946,13 @@
       </c>
     </row>
     <row r="37" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F37" t="s">
@@ -2600,13 +2960,13 @@
       </c>
     </row>
     <row r="38" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F38" t="s">
@@ -2614,13 +2974,13 @@
       </c>
     </row>
     <row r="39" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F39" t="s">
@@ -2628,13 +2988,13 @@
       </c>
     </row>
     <row r="40" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F40" t="s">
@@ -2642,13 +3002,13 @@
       </c>
     </row>
     <row r="41" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F41" t="s">
@@ -2656,13 +3016,13 @@
       </c>
     </row>
     <row r="42" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F42" t="s">
@@ -2673,13 +3033,13 @@
       </c>
     </row>
     <row r="43" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F43" t="s">
@@ -2690,13 +3050,13 @@
       </c>
     </row>
     <row r="44" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F44" t="s">
@@ -2707,13 +3067,13 @@
       </c>
     </row>
     <row r="45" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F45" t="s">
@@ -2724,13 +3084,13 @@
       </c>
     </row>
     <row r="46" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F46" t="s">
@@ -2741,13 +3101,13 @@
       </c>
     </row>
     <row r="47" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F47" t="s">
@@ -2758,13 +3118,13 @@
       </c>
     </row>
     <row r="48" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F48" t="s">
@@ -2772,13 +3132,13 @@
       </c>
     </row>
     <row r="49" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F49" t="s">
@@ -2789,13 +3149,13 @@
       </c>
     </row>
     <row r="50" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F50" t="s">
@@ -2803,13 +3163,13 @@
       </c>
     </row>
     <row r="51" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F51" t="s">
@@ -2820,13 +3180,13 @@
       </c>
     </row>
     <row r="52" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F52" t="s">
@@ -2834,13 +3194,13 @@
       </c>
     </row>
     <row r="53" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F53" t="s">
@@ -2851,13 +3211,13 @@
       </c>
     </row>
     <row r="54" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F54" t="s">
@@ -2865,13 +3225,13 @@
       </c>
     </row>
     <row r="55" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F55" t="s">
@@ -2882,13 +3242,13 @@
       </c>
     </row>
     <row r="56" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F56" t="s">
@@ -2896,13 +3256,13 @@
       </c>
     </row>
     <row r="57" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F57" t="s">
@@ -2913,13 +3273,13 @@
       </c>
     </row>
     <row r="58" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F58" t="s">
@@ -2927,13 +3287,13 @@
       </c>
     </row>
     <row r="59" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F59" t="s">
@@ -2944,13 +3304,13 @@
       </c>
     </row>
     <row r="60" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F60" t="s">
@@ -2958,13 +3318,13 @@
       </c>
     </row>
     <row r="61" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F61" t="s">
@@ -2975,13 +3335,13 @@
       </c>
     </row>
     <row r="62" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F62" t="s">
@@ -2989,13 +3349,13 @@
       </c>
     </row>
     <row r="63" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F63" t="s">
@@ -3003,13 +3363,13 @@
       </c>
     </row>
     <row r="64" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F64" t="s">
@@ -3017,13 +3377,13 @@
       </c>
     </row>
     <row r="65" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F65" t="s">
@@ -3031,13 +3391,13 @@
       </c>
     </row>
     <row r="66" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F66" t="s">
@@ -3045,13 +3405,13 @@
       </c>
     </row>
     <row r="67" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F67" t="s">
@@ -3062,13 +3422,13 @@
       </c>
     </row>
     <row r="68" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F68" t="s">
@@ -3079,13 +3439,13 @@
       </c>
     </row>
     <row r="69" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F69" t="s">
@@ -3096,13 +3456,13 @@
       </c>
     </row>
     <row r="70" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" s="2" t="s">
         <v>175</v>
       </c>
       <c r="F70" t="s">
@@ -3113,13 +3473,13 @@
       </c>
     </row>
     <row r="71" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" s="2" t="s">
         <v>175</v>
       </c>
       <c r="F71" t="s">
@@ -3130,13 +3490,13 @@
       </c>
     </row>
     <row r="72" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="2" t="s">
         <v>175</v>
       </c>
       <c r="F72" t="s">
@@ -3147,13 +3507,13 @@
       </c>
     </row>
     <row r="73" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" s="2" t="s">
         <v>175</v>
       </c>
       <c r="F73" t="s">
@@ -3164,13 +3524,13 @@
       </c>
     </row>
     <row r="74" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" s="2" t="s">
         <v>175</v>
       </c>
       <c r="F74" t="s">
@@ -3181,13 +3541,13 @@
       </c>
     </row>
     <row r="75" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C75" s="4" t="s">
+      <c r="C75" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E75" s="4" t="s">
+      <c r="E75" s="2" t="s">
         <v>175</v>
       </c>
       <c r="F75" t="s">
@@ -3198,13 +3558,13 @@
       </c>
     </row>
     <row r="76" spans="3:7" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E76" s="4" t="s">
+      <c r="E76" s="2" t="s">
         <v>184</v>
       </c>
       <c r="F76" t="s">
@@ -3212,13 +3572,13 @@
       </c>
     </row>
     <row r="77" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C77" s="4" t="s">
+      <c r="C77" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D77" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E77" s="4" t="s">
+      <c r="E77" s="2" t="s">
         <v>188</v>
       </c>
       <c r="F77" t="s">
@@ -3226,13 +3586,13 @@
       </c>
     </row>
     <row r="78" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="2" t="s">
         <v>192</v>
       </c>
       <c r="F78" t="s">
@@ -3240,13 +3600,13 @@
       </c>
     </row>
     <row r="79" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C79" s="4" t="s">
+      <c r="C79" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D79" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E79" s="4" t="s">
+      <c r="E79" s="2" t="s">
         <v>196</v>
       </c>
       <c r="F79" t="s">
@@ -3257,13 +3617,13 @@
       </c>
     </row>
     <row r="80" spans="3:7" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E80" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F80" t="s">
@@ -3274,13 +3634,13 @@
       </c>
     </row>
     <row r="81" spans="3:7" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F81" t="s">
@@ -3291,13 +3651,13 @@
       </c>
     </row>
     <row r="82" spans="3:7" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D82" s="4" t="s">
+      <c r="D82" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E82" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F82" t="s">
@@ -3308,13 +3668,13 @@
       </c>
     </row>
     <row r="83" spans="3:7" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C83" s="4" t="s">
+      <c r="C83" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D83" s="4" t="s">
+      <c r="D83" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E83" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F83" t="s">
@@ -3325,13 +3685,13 @@
       </c>
     </row>
     <row r="84" spans="3:7" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D84" s="4" t="s">
+      <c r="D84" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E84" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F84" t="s">
@@ -3342,13 +3702,13 @@
       </c>
     </row>
     <row r="85" spans="3:7" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="D85" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F85" t="s">
@@ -3359,13 +3719,13 @@
       </c>
     </row>
     <row r="86" spans="3:7" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D86" s="4" t="s">
+      <c r="D86" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F86" t="s">
@@ -3376,13 +3736,13 @@
       </c>
     </row>
     <row r="87" spans="3:7" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C87" s="4" t="s">
+      <c r="C87" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E87" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F87" t="s">
@@ -3393,13 +3753,13 @@
       </c>
     </row>
     <row r="88" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C88" s="4" t="s">
+      <c r="C88" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E88" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F88" t="s">
@@ -3410,13 +3770,13 @@
       </c>
     </row>
     <row r="89" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E89" s="4" t="s">
+      <c r="E89" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F89" t="s">
@@ -3427,13 +3787,13 @@
       </c>
     </row>
     <row r="90" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="D90" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E90" s="4" t="s">
+      <c r="E90" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F90" t="s">
@@ -3444,13 +3804,13 @@
       </c>
     </row>
     <row r="91" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="D91" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E91" s="4" t="s">
+      <c r="E91" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F91" t="s">
@@ -3461,13 +3821,13 @@
       </c>
     </row>
     <row r="92" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C92" s="4" t="s">
+      <c r="C92" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="E92" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F92" t="s">
@@ -3478,13 +3838,13 @@
       </c>
     </row>
     <row r="93" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C93" s="4" t="s">
+      <c r="C93" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E93" s="4" t="s">
+      <c r="E93" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F93" t="s">
@@ -3495,13 +3855,13 @@
       </c>
     </row>
     <row r="94" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E94" s="4" t="s">
+      <c r="E94" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F94" t="s">
@@ -3512,13 +3872,13 @@
       </c>
     </row>
     <row r="95" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C95" s="4" t="s">
+      <c r="C95" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E95" s="4" t="s">
+      <c r="E95" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F95" t="s">
@@ -3529,13 +3889,13 @@
       </c>
     </row>
     <row r="96" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D96" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E96" s="4" t="s">
+      <c r="E96" s="2" t="s">
         <v>188</v>
       </c>
       <c r="F96" t="s">
@@ -3543,13 +3903,13 @@
       </c>
     </row>
     <row r="97" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C97" s="4" t="s">
+      <c r="C97" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D97" s="4" t="s">
+      <c r="D97" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E97" s="4" t="s">
+      <c r="E97" s="2" t="s">
         <v>225</v>
       </c>
       <c r="F97" t="s">
@@ -3560,13 +3920,13 @@
       </c>
     </row>
     <row r="98" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C98" s="4" t="s">
+      <c r="C98" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E98" s="4" t="s">
+      <c r="E98" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F98" t="s">
@@ -3574,13 +3934,13 @@
       </c>
     </row>
     <row r="99" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C99" s="4" t="s">
+      <c r="C99" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D99" s="4" t="s">
+      <c r="D99" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E99" s="4" t="s">
+      <c r="E99" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F99" t="s">
@@ -3588,13 +3948,13 @@
       </c>
     </row>
     <row r="100" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D100" s="4" t="s">
+      <c r="D100" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E100" s="4" t="s">
+      <c r="E100" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F100" t="s">
@@ -3602,13 +3962,13 @@
       </c>
     </row>
     <row r="101" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C101" s="4" t="s">
+      <c r="C101" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D101" s="4" t="s">
+      <c r="D101" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E101" s="4" t="s">
+      <c r="E101" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F101" t="s">
@@ -3616,13 +3976,13 @@
       </c>
     </row>
     <row r="102" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E102" s="4" t="s">
+      <c r="E102" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F102" t="s">
@@ -3630,13 +3990,13 @@
       </c>
     </row>
     <row r="103" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C103" s="4" t="s">
+      <c r="C103" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E103" s="4" t="s">
+      <c r="E103" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F103" t="s">
@@ -3644,13 +4004,13 @@
       </c>
     </row>
     <row r="104" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C104" s="4" t="s">
+      <c r="C104" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E104" s="4" t="s">
+      <c r="E104" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F104" t="s">
@@ -3658,13 +4018,13 @@
       </c>
     </row>
     <row r="105" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C105" s="4" t="s">
+      <c r="C105" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D105" s="4" t="s">
+      <c r="D105" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E105" s="4" t="s">
+      <c r="E105" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F105" t="s">
@@ -3672,13 +4032,13 @@
       </c>
     </row>
     <row r="106" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C106" s="4" t="s">
+      <c r="C106" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D106" s="4" t="s">
+      <c r="D106" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E106" s="4" t="s">
+      <c r="E106" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F106" t="s">
@@ -3686,13 +4046,13 @@
       </c>
     </row>
     <row r="107" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C107" s="4" t="s">
+      <c r="C107" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E107" s="4" t="s">
+      <c r="E107" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F107" t="s">
@@ -3700,13 +4060,13 @@
       </c>
     </row>
     <row r="108" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D108" s="4" t="s">
+      <c r="D108" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E108" s="4" t="s">
+      <c r="E108" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F108" t="s">
@@ -3714,13 +4074,13 @@
       </c>
     </row>
     <row r="109" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C109" s="4" t="s">
+      <c r="C109" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E109" s="4" t="s">
+      <c r="E109" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F109" t="s">
@@ -3728,13 +4088,13 @@
       </c>
     </row>
     <row r="110" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E110" s="4" t="s">
+      <c r="E110" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F110" t="s">
@@ -3742,13 +4102,13 @@
       </c>
     </row>
     <row r="111" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C111" s="4" t="s">
+      <c r="C111" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D111" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E111" s="4" t="s">
+      <c r="E111" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F111" t="s">
@@ -3756,13 +4116,13 @@
       </c>
     </row>
     <row r="112" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C112" s="4" t="s">
+      <c r="C112" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D112" s="4" t="s">
+      <c r="D112" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E112" s="4" t="s">
+      <c r="E112" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F112" t="s">
@@ -3770,13 +4130,13 @@
       </c>
     </row>
     <row r="113" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C113" s="4" t="s">
+      <c r="C113" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D113" s="4" t="s">
+      <c r="D113" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E113" s="4" t="s">
+      <c r="E113" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F113" t="s">
@@ -3784,13 +4144,13 @@
       </c>
     </row>
     <row r="114" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C114" s="4" t="s">
+      <c r="C114" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D114" s="4" t="s">
+      <c r="D114" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E114" s="4" t="s">
+      <c r="E114" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F114" t="s">
@@ -3798,13 +4158,13 @@
       </c>
     </row>
     <row r="115" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C115" s="4" t="s">
+      <c r="C115" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D115" s="4" t="s">
+      <c r="D115" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E115" s="4" t="s">
+      <c r="E115" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F115" t="s">
@@ -3812,13 +4172,13 @@
       </c>
     </row>
     <row r="116" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C116" s="4" t="s">
+      <c r="C116" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D116" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E116" s="4" t="s">
+      <c r="E116" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F116" t="s">
@@ -3826,13 +4186,13 @@
       </c>
     </row>
     <row r="117" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C117" s="4" t="s">
+      <c r="C117" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E117" s="4" t="s">
+      <c r="E117" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F117" t="s">
@@ -3840,13 +4200,13 @@
       </c>
     </row>
     <row r="118" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C118" s="4" t="s">
+      <c r="C118" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D118" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E118" s="4" t="s">
+      <c r="E118" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F118" t="s">
@@ -3854,13 +4214,13 @@
       </c>
     </row>
     <row r="119" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C119" s="4" t="s">
+      <c r="C119" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D119" s="4" t="s">
+      <c r="D119" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E119" s="4" t="s">
+      <c r="E119" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F119" t="s">
@@ -3868,13 +4228,13 @@
       </c>
     </row>
     <row r="120" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C120" s="4" t="s">
+      <c r="C120" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E120" s="4" t="s">
+      <c r="E120" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F120" t="s">
@@ -3882,13 +4242,13 @@
       </c>
     </row>
     <row r="121" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C121" s="4" t="s">
+      <c r="C121" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D121" s="4" t="s">
+      <c r="D121" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E121" s="4" t="s">
+      <c r="E121" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F121" t="s">
@@ -3896,13 +4256,13 @@
       </c>
     </row>
     <row r="122" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C122" s="4" t="s">
+      <c r="C122" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D122" s="4" t="s">
+      <c r="D122" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E122" s="4" t="s">
+      <c r="E122" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F122" t="s">
@@ -3910,13 +4270,13 @@
       </c>
     </row>
     <row r="123" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C123" s="4" t="s">
+      <c r="C123" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D123" s="4" t="s">
+      <c r="D123" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E123" s="4" t="s">
+      <c r="E123" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F123" t="s">
@@ -3924,13 +4284,13 @@
       </c>
     </row>
     <row r="124" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C124" s="4" t="s">
+      <c r="C124" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D124" s="4" t="s">
+      <c r="D124" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E124" s="4" t="s">
+      <c r="E124" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F124" t="s">
@@ -3938,13 +4298,13 @@
       </c>
     </row>
     <row r="125" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C125" s="4" t="s">
+      <c r="C125" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D125" s="4" t="s">
+      <c r="D125" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E125" s="4" t="s">
+      <c r="E125" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F125" t="s">
@@ -3952,13 +4312,13 @@
       </c>
     </row>
     <row r="126" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C126" s="4" t="s">
+      <c r="C126" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D126" s="4" t="s">
+      <c r="D126" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E126" s="4" t="s">
+      <c r="E126" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F126" t="s">
@@ -3966,13 +4326,13 @@
       </c>
     </row>
     <row r="127" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C127" s="4" t="s">
+      <c r="C127" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="D127" s="4" t="s">
+      <c r="D127" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E127" s="4" t="s">
+      <c r="E127" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F127" t="s">
@@ -3980,13 +4340,13 @@
       </c>
     </row>
     <row r="128" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C128" s="4" t="s">
+      <c r="C128" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D128" s="4" t="s">
+      <c r="D128" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E128" s="4" t="s">
+      <c r="E128" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F128" t="s">
@@ -3997,13 +4357,13 @@
       </c>
     </row>
     <row r="129" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C129" s="4" t="s">
+      <c r="C129" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D129" s="4" t="s">
+      <c r="D129" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="E129" s="4" t="s">
+      <c r="E129" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F129" t="s">
@@ -4014,13 +4374,13 @@
       </c>
     </row>
     <row r="130" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C130" s="4" t="s">
+      <c r="C130" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="D130" s="4" t="s">
+      <c r="D130" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="E130" s="4" t="s">
+      <c r="E130" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F130" t="s">
@@ -4031,13 +4391,13 @@
       </c>
     </row>
     <row r="131" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C131" s="4" t="s">
+      <c r="C131" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D131" s="4" t="s">
+      <c r="D131" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E131" s="4" t="s">
+      <c r="E131" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F131" t="s">
@@ -4048,13 +4408,13 @@
       </c>
     </row>
     <row r="132" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C132" s="4" t="s">
+      <c r="C132" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D132" s="4" t="s">
+      <c r="D132" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E132" s="4" t="s">
+      <c r="E132" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F132" t="s">
@@ -4065,13 +4425,13 @@
       </c>
     </row>
     <row r="133" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C133" s="4" t="s">
+      <c r="C133" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="D133" s="4" t="s">
+      <c r="D133" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E133" s="4" t="s">
+      <c r="E133" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F133" t="s">
@@ -4079,13 +4439,13 @@
       </c>
     </row>
     <row r="134" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C134" s="4" t="s">
+      <c r="C134" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="D134" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E134" s="4" t="s">
+      <c r="E134" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F134" t="s">
@@ -4093,13 +4453,13 @@
       </c>
     </row>
     <row r="135" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C135" s="4" t="s">
+      <c r="C135" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="D135" s="4" t="s">
+      <c r="D135" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E135" s="4" t="s">
+      <c r="E135" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F135" t="s">
@@ -4107,13 +4467,13 @@
       </c>
     </row>
     <row r="136" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C136" s="4" t="s">
+      <c r="C136" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="D136" s="4" t="s">
+      <c r="D136" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E136" s="4" t="s">
+      <c r="E136" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F136" t="s">
@@ -4121,13 +4481,13 @@
       </c>
     </row>
     <row r="137" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C137" s="4" t="s">
+      <c r="C137" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="D137" s="4" t="s">
+      <c r="D137" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E137" s="4" t="s">
+      <c r="E137" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F137" t="s">
@@ -4138,13 +4498,13 @@
       </c>
     </row>
     <row r="138" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C138" s="4" t="s">
+      <c r="C138" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="D138" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E138" s="4" t="s">
+      <c r="E138" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F138" t="s">
@@ -4152,13 +4512,13 @@
       </c>
     </row>
     <row r="139" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C139" s="4" t="s">
+      <c r="C139" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="D139" s="4" t="s">
+      <c r="D139" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E139" s="4" t="s">
+      <c r="E139" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F139" t="s">
@@ -4166,13 +4526,13 @@
       </c>
     </row>
     <row r="140" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C140" s="4" t="s">
+      <c r="C140" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D140" s="4" t="s">
+      <c r="D140" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E140" s="4" t="s">
+      <c r="E140" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F140" t="s">
@@ -4180,13 +4540,13 @@
       </c>
     </row>
     <row r="141" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C141" s="4" t="s">
+      <c r="C141" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="D141" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E141" s="4" t="s">
+      <c r="E141" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F141" t="s">
@@ -4194,13 +4554,13 @@
       </c>
     </row>
     <row r="142" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C142" s="4" t="s">
+      <c r="C142" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D142" s="4" t="s">
+      <c r="D142" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E142" s="4" t="s">
+      <c r="E142" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F142" t="s">
@@ -4211,13 +4571,13 @@
       </c>
     </row>
     <row r="143" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C143" s="4" t="s">
+      <c r="C143" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="D143" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E143" s="4" t="s">
+      <c r="E143" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F143" t="s">
@@ -4225,13 +4585,13 @@
       </c>
     </row>
     <row r="144" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C144" s="4" t="s">
+      <c r="C144" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="D144" s="4" t="s">
+      <c r="D144" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E144" s="4" t="s">
+      <c r="E144" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F144" t="s">
@@ -4239,13 +4599,13 @@
       </c>
     </row>
     <row r="145" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C145" s="4" t="s">
+      <c r="C145" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D145" s="4" t="s">
+      <c r="D145" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E145" s="4" t="s">
+      <c r="E145" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F145" t="s">
@@ -4253,13 +4613,13 @@
       </c>
     </row>
     <row r="146" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C146" s="4" t="s">
+      <c r="C146" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D146" s="4" t="s">
+      <c r="D146" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E146" s="4" t="s">
+      <c r="E146" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F146" t="s">
@@ -4267,13 +4627,13 @@
       </c>
     </row>
     <row r="147" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C147" s="4" t="s">
+      <c r="C147" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="D147" s="4" t="s">
+      <c r="D147" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E147" s="4" t="s">
+      <c r="E147" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F147" t="s">
@@ -4284,13 +4644,13 @@
       </c>
     </row>
     <row r="148" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C148" s="4" t="s">
+      <c r="C148" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D148" s="4" t="s">
+      <c r="D148" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E148" s="4" t="s">
+      <c r="E148" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F148" t="s">
@@ -4298,13 +4658,13 @@
       </c>
     </row>
     <row r="149" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C149" s="4" t="s">
+      <c r="C149" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D149" s="4" t="s">
+      <c r="D149" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E149" s="4" t="s">
+      <c r="E149" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F149" t="s">
@@ -4312,13 +4672,13 @@
       </c>
     </row>
     <row r="150" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C150" s="4" t="s">
+      <c r="C150" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D150" s="4" t="s">
+      <c r="D150" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E150" s="4" t="s">
+      <c r="E150" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F150" t="s">
@@ -4326,13 +4686,13 @@
       </c>
     </row>
     <row r="151" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C151" s="4" t="s">
+      <c r="C151" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D151" s="4" t="s">
+      <c r="D151" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E151" s="4" t="s">
+      <c r="E151" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F151" t="s">
@@ -4340,13 +4700,13 @@
       </c>
     </row>
     <row r="152" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C152" s="4" t="s">
+      <c r="C152" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D152" s="4" t="s">
+      <c r="D152" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E152" s="4" t="s">
+      <c r="E152" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F152" t="s">
@@ -4357,13 +4717,13 @@
       </c>
     </row>
     <row r="153" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C153" s="4" t="s">
+      <c r="C153" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D153" s="4" t="s">
+      <c r="D153" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E153" s="4" t="s">
+      <c r="E153" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F153" t="s">
@@ -4371,13 +4731,13 @@
       </c>
     </row>
     <row r="154" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C154" s="4" t="s">
+      <c r="C154" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D154" s="4" t="s">
+      <c r="D154" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E154" s="4" t="s">
+      <c r="E154" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F154" t="s">
@@ -4385,13 +4745,13 @@
       </c>
     </row>
     <row r="155" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C155" s="4" t="s">
+      <c r="C155" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D155" s="4" t="s">
+      <c r="D155" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E155" s="4" t="s">
+      <c r="E155" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F155" t="s">
@@ -4399,13 +4759,13 @@
       </c>
     </row>
     <row r="156" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C156" s="4" t="s">
+      <c r="C156" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D156" s="4" t="s">
+      <c r="D156" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E156" s="4" t="s">
+      <c r="E156" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F156" t="s">
@@ -4413,13 +4773,13 @@
       </c>
     </row>
     <row r="157" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C157" s="4" t="s">
+      <c r="C157" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D157" s="4" t="s">
+      <c r="D157" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E157" s="4" t="s">
+      <c r="E157" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F157" t="s">
@@ -4430,13 +4790,13 @@
       </c>
     </row>
     <row r="158" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C158" s="4" t="s">
+      <c r="C158" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D158" s="4" t="s">
+      <c r="D158" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E158" s="4" t="s">
+      <c r="E158" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F158" t="s">
@@ -4444,13 +4804,13 @@
       </c>
     </row>
     <row r="159" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C159" s="4" t="s">
+      <c r="C159" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D159" s="4" t="s">
+      <c r="D159" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E159" s="4" t="s">
+      <c r="E159" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F159" t="s">
@@ -4458,13 +4818,13 @@
       </c>
     </row>
     <row r="160" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C160" s="4" t="s">
+      <c r="C160" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D160" s="4" t="s">
+      <c r="D160" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E160" s="4" t="s">
+      <c r="E160" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F160" t="s">
@@ -4472,13 +4832,13 @@
       </c>
     </row>
     <row r="161" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C161" s="4" t="s">
+      <c r="C161" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D161" s="4" t="s">
+      <c r="D161" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E161" s="4" t="s">
+      <c r="E161" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F161" t="s">
@@ -4486,13 +4846,13 @@
       </c>
     </row>
     <row r="162" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C162" s="4" t="s">
+      <c r="C162" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D162" s="4" t="s">
+      <c r="D162" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E162" s="4" t="s">
+      <c r="E162" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F162" t="s">
@@ -4503,13 +4863,13 @@
       </c>
     </row>
     <row r="163" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C163" s="4" t="s">
+      <c r="C163" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D163" s="4" t="s">
+      <c r="D163" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E163" s="4" t="s">
+      <c r="E163" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F163" t="s">
@@ -4517,13 +4877,13 @@
       </c>
     </row>
     <row r="164" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C164" s="4" t="s">
+      <c r="C164" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D164" s="4" t="s">
+      <c r="D164" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E164" s="4" t="s">
+      <c r="E164" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F164" t="s">
@@ -4531,13 +4891,13 @@
       </c>
     </row>
     <row r="165" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C165" s="4" t="s">
+      <c r="C165" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D165" s="4" t="s">
+      <c r="D165" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E165" s="4" t="s">
+      <c r="E165" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F165" t="s">
@@ -4545,13 +4905,13 @@
       </c>
     </row>
     <row r="166" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C166" s="4" t="s">
+      <c r="C166" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D166" s="4" t="s">
+      <c r="D166" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E166" s="4" t="s">
+      <c r="E166" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F166" t="s">
@@ -4559,13 +4919,13 @@
       </c>
     </row>
     <row r="167" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C167" s="4" t="s">
+      <c r="C167" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D167" s="4" t="s">
+      <c r="D167" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E167" s="4" t="s">
+      <c r="E167" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F167" t="s">
@@ -4576,13 +4936,13 @@
       </c>
     </row>
     <row r="168" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C168" s="4" t="s">
+      <c r="C168" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D168" s="4" t="s">
+      <c r="D168" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E168" s="4" t="s">
+      <c r="E168" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F168" t="s">
@@ -4590,13 +4950,13 @@
       </c>
     </row>
     <row r="169" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C169" s="4" t="s">
+      <c r="C169" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D169" s="4" t="s">
+      <c r="D169" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E169" s="4" t="s">
+      <c r="E169" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F169" t="s">
@@ -4604,13 +4964,13 @@
       </c>
     </row>
     <row r="170" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C170" s="4" t="s">
+      <c r="C170" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D170" s="4" t="s">
+      <c r="D170" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E170" s="4" t="s">
+      <c r="E170" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F170" t="s">
@@ -4618,13 +4978,13 @@
       </c>
     </row>
     <row r="171" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C171" s="4" t="s">
+      <c r="C171" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D171" s="4" t="s">
+      <c r="D171" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E171" s="4" t="s">
+      <c r="E171" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F171" t="s">
@@ -4632,13 +4992,13 @@
       </c>
     </row>
     <row r="172" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C172" s="4" t="s">
+      <c r="C172" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D172" s="4" t="s">
+      <c r="D172" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E172" s="4" t="s">
+      <c r="E172" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F172" t="s">
@@ -4649,13 +5009,13 @@
       </c>
     </row>
     <row r="173" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C173" s="4" t="s">
+      <c r="C173" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D173" s="4">
+      <c r="D173" s="2">
         <v>220</v>
       </c>
-      <c r="E173" s="4" t="s">
+      <c r="E173" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F173" t="s">
@@ -4663,13 +5023,13 @@
       </c>
     </row>
     <row r="174" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C174" s="4" t="s">
+      <c r="C174" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D174" s="4">
+      <c r="D174" s="2">
         <v>220</v>
       </c>
-      <c r="E174" s="4" t="s">
+      <c r="E174" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F174" t="s">
@@ -4677,13 +5037,13 @@
       </c>
     </row>
     <row r="175" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C175" s="4" t="s">
+      <c r="C175" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D175" s="2">
         <v>220</v>
       </c>
-      <c r="E175" s="4" t="s">
+      <c r="E175" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F175" t="s">
@@ -4691,13 +5051,13 @@
       </c>
     </row>
     <row r="176" spans="3:7" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C176" s="4" t="s">
+      <c r="C176" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D176" s="2">
         <v>220</v>
       </c>
-      <c r="E176" s="4" t="s">
+      <c r="E176" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F176" t="s">
@@ -4705,13 +5065,13 @@
       </c>
     </row>
     <row r="177" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C177" s="4" t="s">
+      <c r="C177" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D177" s="4" t="s">
+      <c r="D177" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E177" s="4" t="s">
+      <c r="E177" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F177" t="s">
@@ -4743,13 +5103,13 @@
       </c>
     </row>
     <row r="178" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C178" s="4" t="s">
+      <c r="C178" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D178" s="4" t="s">
+      <c r="D178" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E178" s="4" t="s">
+      <c r="E178" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F178" t="s">
@@ -4781,13 +5141,13 @@
       </c>
     </row>
     <row r="179" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C179" s="4" t="s">
+      <c r="C179" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D179" s="4" t="s">
+      <c r="D179" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E179" s="4" t="s">
+      <c r="E179" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F179" t="s">
@@ -4819,13 +5179,13 @@
       </c>
     </row>
     <row r="180" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C180" s="4" t="s">
+      <c r="C180" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="D180" s="4" t="s">
+      <c r="D180" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E180" s="4" t="s">
+      <c r="E180" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F180" t="s">
@@ -4857,13 +5217,13 @@
       </c>
     </row>
     <row r="181" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C181" s="4" t="s">
+      <c r="C181" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D181" s="4" t="s">
+      <c r="D181" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E181" s="4" t="s">
+      <c r="E181" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F181" t="s">
@@ -4895,13 +5255,13 @@
       </c>
     </row>
     <row r="182" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C182" s="4" t="s">
+      <c r="C182" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D182" s="4" t="s">
+      <c r="D182" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E182" s="4" t="s">
+      <c r="E182" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F182" t="s">
@@ -4933,13 +5293,13 @@
       </c>
     </row>
     <row r="183" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C183" s="4" t="s">
+      <c r="C183" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D183" s="4" t="s">
+      <c r="D183" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E183" s="4" t="s">
+      <c r="E183" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F183" t="s">
@@ -4971,13 +5331,13 @@
       </c>
     </row>
     <row r="184" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C184" s="4" t="s">
+      <c r="C184" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="D184" s="4" t="s">
+      <c r="D184" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E184" s="4" t="s">
+      <c r="E184" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F184" t="s">
@@ -5009,13 +5369,13 @@
       </c>
     </row>
     <row r="185" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C185" s="4" t="s">
+      <c r="C185" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D185" s="4" t="s">
+      <c r="D185" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="E185" s="4" t="s">
+      <c r="E185" s="2" t="s">
         <v>345</v>
       </c>
       <c r="F185" t="s">
@@ -5026,13 +5386,13 @@
       </c>
     </row>
     <row r="186" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C186" s="4" t="s">
+      <c r="C186" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="D186" s="4" t="s">
+      <c r="D186" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="E186" s="4" t="s">
+      <c r="E186" s="2" t="s">
         <v>349</v>
       </c>
       <c r="F186" t="s">
@@ -5043,13 +5403,13 @@
       </c>
     </row>
     <row r="187" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C187" s="4" t="s">
+      <c r="C187" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="D187" s="4" t="s">
+      <c r="D187" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="E187" s="4" t="s">
+      <c r="E187" s="2" t="s">
         <v>354</v>
       </c>
       <c r="F187" t="s">
@@ -5060,13 +5420,13 @@
       </c>
     </row>
     <row r="188" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C188" s="4" t="s">
+      <c r="C188" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="D188" s="4" t="s">
+      <c r="D188" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="E188" s="4" t="s">
+      <c r="E188" s="2" t="s">
         <v>359</v>
       </c>
       <c r="F188" t="s">
@@ -5077,13 +5437,13 @@
       </c>
     </row>
     <row r="189" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C189" s="4" t="s">
+      <c r="C189" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D189" s="4" t="s">
+      <c r="D189" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="E189" s="4" t="s">
+      <c r="E189" s="2" t="s">
         <v>364</v>
       </c>
       <c r="F189" t="s">
@@ -5091,13 +5451,13 @@
       </c>
     </row>
     <row r="190" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C190" s="4" t="s">
+      <c r="C190" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="D190" s="4" t="s">
+      <c r="D190" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E190" s="4" t="s">
+      <c r="E190" s="2" t="s">
         <v>368</v>
       </c>
       <c r="F190" t="s">
@@ -5108,13 +5468,13 @@
       </c>
     </row>
     <row r="191" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C191" s="4" t="s">
+      <c r="C191" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="D191" s="4" t="s">
+      <c r="D191" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="E191" s="4" t="s">
+      <c r="E191" s="2" t="s">
         <v>371</v>
       </c>
       <c r="F191" t="s">
@@ -5125,13 +5485,13 @@
       </c>
     </row>
     <row r="192" spans="3:14" hidden="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C192" s="4" t="s">
+      <c r="C192" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D192" s="4" t="s">
+      <c r="D192" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E192" s="4" t="s">
+      <c r="E192" s="2" t="s">
         <v>376</v>
       </c>
       <c r="F192" t="s">
@@ -5145,32 +5505,32 @@
     <row r="194" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="196" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A196" s="16" t="s">
+      <c r="A196" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="B196" s="17"/>
-      <c r="C196" s="18"/>
-      <c r="D196" s="18"/>
-      <c r="E196" s="18"/>
-      <c r="F196" s="17"/>
+      <c r="B196" s="7"/>
+      <c r="C196" s="8"/>
+      <c r="D196" s="8"/>
+      <c r="E196" s="8"/>
+      <c r="F196" s="7"/>
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A197" s="17" t="s">
+      <c r="A197" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B197" s="17" t="s">
+      <c r="B197" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C197" s="18" t="s">
+      <c r="C197" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D197" s="18" t="s">
+      <c r="D197" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E197" s="18" t="s">
+      <c r="E197" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F197" s="17" t="s">
+      <c r="F197" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G197" t="s">
@@ -5205,13 +5565,13 @@
       <c r="B198">
         <v>2</v>
       </c>
-      <c r="C198" s="4" t="s">
+      <c r="C198" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="D198" s="4" t="s">
+      <c r="D198" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E198" s="4" t="s">
+      <c r="E198" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F198" t="s">
@@ -5228,13 +5588,13 @@
       <c r="B199">
         <v>13</v>
       </c>
-      <c r="C199" s="4" t="s">
+      <c r="C199" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="D199" s="4" t="s">
+      <c r="D199" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E199" s="4" t="s">
+      <c r="E199" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F199" t="s">
@@ -5251,13 +5611,13 @@
       <c r="B200">
         <v>13</v>
       </c>
-      <c r="C200" s="4" t="s">
+      <c r="C200" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="D200" s="4" t="s">
+      <c r="D200" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E200" s="4" t="s">
+      <c r="E200" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F200" t="s">
@@ -5274,13 +5634,13 @@
       <c r="B201">
         <v>2</v>
       </c>
-      <c r="C201" s="4" t="s">
+      <c r="C201" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="D201" s="4" t="s">
+      <c r="D201" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E201" s="4" t="s">
+      <c r="E201" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F201" t="s">
@@ -5297,13 +5657,13 @@
       <c r="B202">
         <v>2</v>
       </c>
-      <c r="C202" s="4" t="s">
+      <c r="C202" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="D202" s="4" t="s">
+      <c r="D202" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E202" s="4" t="s">
+      <c r="E202" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F202" t="s">
@@ -5317,13 +5677,13 @@
       <c r="B203">
         <v>16</v>
       </c>
-      <c r="C203" s="4" t="s">
+      <c r="C203" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="D203" s="4" t="s">
+      <c r="D203" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E203" s="4" t="s">
+      <c r="E203" s="2" t="s">
         <v>136</v>
       </c>
       <c r="F203" t="s">
@@ -5340,13 +5700,13 @@
       <c r="B204">
         <v>1</v>
       </c>
-      <c r="C204" s="4" t="s">
+      <c r="C204" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D204" s="4" t="s">
+      <c r="D204" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E204" s="4" t="s">
+      <c r="E204" s="2" t="s">
         <v>143</v>
       </c>
       <c r="F204" t="s">
@@ -5363,13 +5723,13 @@
       <c r="B205">
         <v>8</v>
       </c>
-      <c r="C205" s="4" t="s">
+      <c r="C205" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="D205" s="4" t="s">
+      <c r="D205" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E205" s="4" t="s">
+      <c r="E205" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F205" t="s">
@@ -5383,13 +5743,13 @@
       <c r="B206">
         <v>3</v>
       </c>
-      <c r="C206" s="4" t="s">
+      <c r="C206" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="D206" s="4" t="s">
+      <c r="D206" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E206" s="4" t="s">
+      <c r="E206" s="2" t="s">
         <v>169</v>
       </c>
       <c r="F206" t="s">
@@ -5406,13 +5766,13 @@
       <c r="B207">
         <v>6</v>
       </c>
-      <c r="C207" s="4" t="s">
+      <c r="C207" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D207" s="4" t="s">
+      <c r="D207" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E207" s="4" t="s">
+      <c r="E207" s="2" t="s">
         <v>175</v>
       </c>
       <c r="F207" t="s">
@@ -5429,13 +5789,13 @@
       <c r="B208">
         <v>1</v>
       </c>
-      <c r="C208" s="4" t="s">
+      <c r="C208" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D208" s="4" t="s">
+      <c r="D208" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E208" s="4" t="s">
+      <c r="E208" s="2" t="s">
         <v>184</v>
       </c>
       <c r="F208" t="s">
@@ -5449,13 +5809,13 @@
       <c r="B209">
         <v>1</v>
       </c>
-      <c r="C209" s="4" t="s">
+      <c r="C209" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D209" s="4" t="s">
+      <c r="D209" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E209" s="4" t="s">
+      <c r="E209" s="2" t="s">
         <v>188</v>
       </c>
       <c r="F209" t="s">
@@ -5469,13 +5829,13 @@
       <c r="B210">
         <v>1</v>
       </c>
-      <c r="C210" s="4" t="s">
+      <c r="C210" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D210" s="4" t="s">
+      <c r="D210" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E210" s="4" t="s">
+      <c r="E210" s="2" t="s">
         <v>192</v>
       </c>
       <c r="F210" t="s">
@@ -5489,13 +5849,13 @@
       <c r="B211">
         <v>1</v>
       </c>
-      <c r="C211" s="4" t="s">
+      <c r="C211" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D211" s="4" t="s">
+      <c r="D211" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E211" s="4" t="s">
+      <c r="E211" s="2" t="s">
         <v>196</v>
       </c>
       <c r="F211" t="s">
@@ -5512,13 +5872,13 @@
       <c r="B212">
         <v>8</v>
       </c>
-      <c r="C212" s="4" t="s">
+      <c r="C212" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="D212" s="4" t="s">
+      <c r="D212" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E212" s="4" t="s">
+      <c r="E212" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F212" t="s">
@@ -5535,13 +5895,13 @@
       <c r="B213">
         <v>8</v>
       </c>
-      <c r="C213" s="4" t="s">
+      <c r="C213" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D213" s="4" t="s">
+      <c r="D213" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E213" s="4" t="s">
+      <c r="E213" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F213" t="s">
@@ -5558,13 +5918,13 @@
       <c r="B214">
         <v>1</v>
       </c>
-      <c r="C214" s="4" t="s">
+      <c r="C214" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D214" s="4" t="s">
+      <c r="D214" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E214" s="4" t="s">
+      <c r="E214" s="2" t="s">
         <v>188</v>
       </c>
       <c r="F214" t="s">
@@ -5578,13 +5938,13 @@
       <c r="B215">
         <v>1</v>
       </c>
-      <c r="C215" s="4" t="s">
+      <c r="C215" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D215" s="4" t="s">
+      <c r="D215" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E215" s="4" t="s">
+      <c r="E215" s="2" t="s">
         <v>225</v>
       </c>
       <c r="F215" t="s">
@@ -5601,13 +5961,13 @@
       <c r="B216">
         <v>8</v>
       </c>
-      <c r="C216" s="4" t="s">
+      <c r="C216" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="D216" s="4" t="s">
+      <c r="D216" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E216" s="4" t="s">
+      <c r="E216" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F216" t="s">
@@ -5621,33 +5981,33 @@
       <c r="B217">
         <v>8</v>
       </c>
-      <c r="C217" s="4" t="s">
+      <c r="C217" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="D217" s="4" t="s">
+      <c r="D217" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E217" s="4" t="s">
+      <c r="E217" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F217" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:7" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A218">
         <v>21</v>
       </c>
       <c r="B218">
         <v>49</v>
       </c>
-      <c r="C218" s="4" t="s">
+      <c r="C218" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="D218" s="4" t="s">
+      <c r="D218" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E218" s="4" t="s">
+      <c r="E218" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F218" t="s">
@@ -5664,13 +6024,13 @@
       <c r="B219">
         <v>4</v>
       </c>
-      <c r="C219" s="4" t="s">
+      <c r="C219" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="D219" s="4" t="s">
+      <c r="D219" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E219" s="4" t="s">
+      <c r="E219" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F219" t="s">
@@ -5684,13 +6044,13 @@
       <c r="B220">
         <v>1</v>
       </c>
-      <c r="C220" s="4" t="s">
+      <c r="C220" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D220" s="4" t="s">
+      <c r="D220" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E220" s="4" t="s">
+      <c r="E220" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F220" t="s">
@@ -5704,13 +6064,13 @@
       <c r="B221">
         <v>1</v>
       </c>
-      <c r="C221" s="4" t="s">
+      <c r="C221" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D221" s="4" t="s">
+      <c r="D221" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E221" s="4" t="s">
+      <c r="E221" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F221" t="s">
@@ -5724,13 +6084,13 @@
       <c r="B222">
         <v>1</v>
       </c>
-      <c r="C222" s="4" t="s">
+      <c r="C222" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D222" s="4" t="s">
+      <c r="D222" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E222" s="4" t="s">
+      <c r="E222" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F222" t="s">
@@ -5747,13 +6107,13 @@
       <c r="B223">
         <v>1</v>
       </c>
-      <c r="C223" s="4" t="s">
+      <c r="C223" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D223" s="4" t="s">
+      <c r="D223" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="E223" s="4" t="s">
+      <c r="E223" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F223" t="s">
@@ -5770,13 +6130,13 @@
       <c r="B224">
         <v>1</v>
       </c>
-      <c r="C224" s="4" t="s">
+      <c r="C224" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="D224" s="4" t="s">
+      <c r="D224" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="E224" s="4" t="s">
+      <c r="E224" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F224" t="s">
@@ -5793,13 +6153,13 @@
       <c r="B225">
         <v>1</v>
       </c>
-      <c r="C225" s="4" t="s">
+      <c r="C225" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D225" s="4" t="s">
+      <c r="D225" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E225" s="4" t="s">
+      <c r="E225" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F225" t="s">
@@ -5816,13 +6176,13 @@
       <c r="B226">
         <v>4</v>
       </c>
-      <c r="C226" s="4" t="s">
+      <c r="C226" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="D226" s="19">
+      <c r="D226" s="9">
         <v>220</v>
       </c>
-      <c r="E226" s="4" t="s">
+      <c r="E226" s="2" t="s">
         <v>252</v>
       </c>
       <c r="F226" t="s">
@@ -5836,13 +6196,13 @@
       <c r="B227">
         <v>8</v>
       </c>
-      <c r="C227" s="4" t="s">
+      <c r="C227" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="D227" s="4" t="s">
+      <c r="D227" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E227" s="4" t="s">
+      <c r="E227" s="2" t="s">
         <v>326</v>
       </c>
       <c r="F227" t="s">
@@ -5880,13 +6240,13 @@
       <c r="B228">
         <v>1</v>
       </c>
-      <c r="C228" s="4" t="s">
+      <c r="C228" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D228" s="4" t="s">
+      <c r="D228" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="E228" s="4" t="s">
+      <c r="E228" s="2" t="s">
         <v>345</v>
       </c>
       <c r="F228" t="s">
@@ -5903,13 +6263,13 @@
       <c r="B229">
         <v>1</v>
       </c>
-      <c r="C229" s="4" t="s">
+      <c r="C229" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="D229" s="4" t="s">
+      <c r="D229" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="E229" s="4" t="s">
+      <c r="E229" s="2" t="s">
         <v>349</v>
       </c>
       <c r="F229" t="s">
@@ -5926,13 +6286,13 @@
       <c r="B230">
         <v>1</v>
       </c>
-      <c r="C230" s="4" t="s">
+      <c r="C230" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="D230" s="4" t="s">
+      <c r="D230" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="E230" s="4" t="s">
+      <c r="E230" s="2" t="s">
         <v>354</v>
       </c>
       <c r="F230" t="s">
@@ -5949,13 +6309,13 @@
       <c r="B231">
         <v>1</v>
       </c>
-      <c r="C231" s="4" t="s">
+      <c r="C231" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="D231" s="4" t="s">
+      <c r="D231" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="E231" s="4" t="s">
+      <c r="E231" s="2" t="s">
         <v>359</v>
       </c>
       <c r="F231" t="s">
@@ -5972,13 +6332,13 @@
       <c r="B232">
         <v>1</v>
       </c>
-      <c r="C232" s="4" t="s">
+      <c r="C232" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D232" s="4" t="s">
+      <c r="D232" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="E232" s="4" t="s">
+      <c r="E232" s="2" t="s">
         <v>364</v>
       </c>
       <c r="F232" t="s">
@@ -5992,13 +6352,13 @@
       <c r="B233">
         <v>1</v>
       </c>
-      <c r="C233" s="4" t="s">
+      <c r="C233" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="D233" s="4" t="s">
+      <c r="D233" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E233" s="4" t="s">
+      <c r="E233" s="2" t="s">
         <v>368</v>
       </c>
       <c r="F233" t="s">
@@ -6015,13 +6375,13 @@
       <c r="B234">
         <v>1</v>
       </c>
-      <c r="C234" s="4" t="s">
+      <c r="C234" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="D234" s="4" t="s">
+      <c r="D234" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="E234" s="4" t="s">
+      <c r="E234" s="2" t="s">
         <v>371</v>
       </c>
       <c r="F234" t="s">
@@ -6038,13 +6398,13 @@
       <c r="B235">
         <v>1</v>
       </c>
-      <c r="C235" s="4" t="s">
+      <c r="C235" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D235" s="4" t="s">
+      <c r="D235" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E235" s="4" t="s">
+      <c r="E235" s="2" t="s">
         <v>376</v>
       </c>
       <c r="F235" t="s">
@@ -6071,11 +6431,283 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5B50BB-9207-4AC4-9E8E-12520AD2311C}">
+  <dimension ref="B1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="H1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="H2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="H3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B4" s="13">
+        <v>28</v>
+      </c>
+      <c r="C4" s="14">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="15">
+        <f>B4*D4/(C4+D4)</f>
+        <v>2.5454545454545454</v>
+      </c>
+      <c r="H4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H5">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="H6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="36" t="s">
+        <v>400</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38" t="s">
+        <v>425</v>
+      </c>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="33" t="s">
+        <v>401</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34">
+        <v>2</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>414</v>
+      </c>
+      <c r="H8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="30" t="s">
+        <v>402</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="29">
+        <v>1</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="I9" t="s">
+        <v>424</v>
+      </c>
+      <c r="J9" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="29">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>422</v>
+      </c>
+      <c r="H10" t="s">
+        <v>411</v>
+      </c>
+      <c r="I10">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="J10">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="29">
+        <v>25</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>416</v>
+      </c>
+      <c r="H11" t="s">
+        <v>412</v>
+      </c>
+      <c r="I11">
+        <v>0.44</v>
+      </c>
+      <c r="J11">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="29">
+        <v>10</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>416</v>
+      </c>
+      <c r="H12" t="s">
+        <v>413</v>
+      </c>
+      <c r="I12">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="J12">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="41">
+        <f>(E8/(IF(D7="External",I10,J10)*E12^I11))^(1/I12)</f>
+        <v>110.28301385119917</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="30" t="s">
+        <v>406</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="41">
+        <f>E13/(E9*1.378)</f>
+        <v>80.031214696080681</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="31" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="31" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="31" t="s">
+        <v>421</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D4" xr:uid="{0B79B1E1-91D8-43EF-8E0D-9B18089F27A7}">
+      <formula1>$H$2:$H$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7" xr:uid="{B442EC8B-096F-45F8-97FE-1A915E91BC94}">
+      <formula1>$I$9:$J$9</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4575EB26-62A7-4BE8-8784-F0F6E443F592}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6093,6 +6725,11 @@
         <v>65</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>426</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>